<commit_message>
se agregan los archivos finales y se actualizan los viejos
</commit_message>
<xml_diff>
--- a/Herramienta matriz de riesgos.xlsx
+++ b/Herramienta matriz de riesgos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andes\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andes\OneDrive\Documentos\ANDRES\semillero\taller_4\2024-C1-QA-FP-T04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410CC3FA-E336-45A9-B9ED-ECFCB3CA7F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12026271-AE25-4096-A8E9-A86A49E1DA25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Definiciones" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Descripcion!$B$2:$P$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Descripcion!$B$2:$O$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -55,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="197">
   <si>
     <t xml:space="preserve">Nombre del responsable </t>
   </si>
@@ -252,9 +252,6 @@
   </si>
   <si>
     <t>Realizar una comunicación efectiva con el cliente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Andreina </t>
   </si>
   <si>
     <t>CBA: 2- Desviacion Presupuesto</t>
@@ -429,19 +426,247 @@
     <t>Sobrecarga del Servidor por Alto Flujo de Usuarios</t>
   </si>
   <si>
-    <t>Cambios de Requisitos del Cliente Impactando en Aumento de Costos</t>
-  </si>
-  <si>
     <t>Desviaciones del Presupuesto durante el Desarrollo del Proyecto</t>
   </si>
   <si>
-    <t>Falta de Experiencia en el Equipo Generando Retrasos y Aumento de Costos</t>
-  </si>
-  <si>
-    <t>Comunicación Deficiente entre los Miembros del Equipo Generando Problemas y Retrasos</t>
-  </si>
-  <si>
-    <t>Conflictos Internos en el Equipo del Proyecto Afectando la Colaboración y Productividad</t>
+    <t>Descripción del Producto Incorrecta</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Es posible que la descripción del producto no sea precisa o esté incompleta, lo que podría llevar a malentendidos por parte de los clientes y a un aumento en las devoluciones.</t>
+  </si>
+  <si>
+    <t>Falta de Imágenes o Imágenes Inadecuadas</t>
+  </si>
+  <si>
+    <t>Información de Stock Errónea</t>
+  </si>
+  <si>
+    <t>Si la información sobre el stock de un producto no se actualiza correctamente, los clientes podrían realizar una compra y luego enterarse de que el producto no está disponible, lo que resultaría en una experiencia insatisfactoria</t>
+  </si>
+  <si>
+    <t>Problemas de Navegación</t>
+  </si>
+  <si>
+    <t>Si la página de Amazon experimenta problemas de navegación, como enlaces rotos o una interfaz confusa, los clientes pueden tener dificultades para encontrar lo que están buscando y optar por comprar en otro lugar</t>
+  </si>
+  <si>
+    <t>Errores en la Funcionalidad del Carrito de Compras</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Los errores en el proceso de compra, como problemas al agregar productos al carrito o al finalizar la compra, pueden resultar en pérdidas de ventas y frustración del cliente</t>
+  </si>
+  <si>
+    <t>Puede que la falta de imágenes o imágenes de baja calidad puede afectar negativamente la experiencia del cliente y reducir las ventas</t>
+  </si>
+  <si>
+    <t>Problemas de Traducción o Localización</t>
+  </si>
+  <si>
+    <t>Si la traducción o localización de la página de Amazon no es precisa, los clientes que hablan diferentes idiomas pueden experimentar dificultades para entender la información del producto y realizar compras.</t>
+  </si>
+  <si>
+    <t>Problemas de Categorización de Productos</t>
+  </si>
+  <si>
+    <t>Una categorización incorrecta de los productos puede dificultar que los clientes encuentren lo que están buscando y reducir la efectividad de las recomendaciones personalizadas</t>
+  </si>
+  <si>
+    <t>Falta de Comentarios de los Clientes</t>
+  </si>
+  <si>
+    <t>La falta de comentarios o reseñas de los clientes puede hacer que los clientes duden en realizar una compra, ya que no tienen información sobre la calidad del producto o la experiencia de otros usuarios</t>
+  </si>
+  <si>
+    <t>Problemas de Carga de Página</t>
+  </si>
+  <si>
+    <t>Si la página de Amazon experimenta tiempos de carga lentos o problemas de rendimiento, los clientes pueden abandonar el sitio antes de completar una compra, lo que resultaría en pérdidas de ventas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cambios de Requisitos del Cliente </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falta de Experiencia en el Equipo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comunicación Deficiente entre los Miembros del Equipo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conflictos Internos en el Equipo del Proyecto </t>
+  </si>
+  <si>
+    <t>Problemas de Gestión del Tiempo</t>
+  </si>
+  <si>
+    <t>La gestión ineficaz del tiempo puede resultar en retrasos en la entrega del proyecto y afectar su viabilidad en el mercado</t>
+  </si>
+  <si>
+    <t>Falta de Planificación Adecuada</t>
+  </si>
+  <si>
+    <t>Una planificación inadecuada del proyecto puede resultar en estimaciones incorrectas, retrasos en la entrega y un aumento de los costos</t>
+  </si>
+  <si>
+    <t>Cambios en la Tecnología</t>
+  </si>
+  <si>
+    <t>Cambios en la tecnología durante el desarrollo del proyecto pueden requerir ajustes en la arquitectura y el diseño, lo que puede causar retrasos y aumentar los costos</t>
+  </si>
+  <si>
+    <t>Problemas de Integración de Sistemas</t>
+  </si>
+  <si>
+    <t>Dificultades para integrar las nuevas funcionalidades con los sistemas existentes de Amazon pueden causar retrasos en el proyecto y afectar la funcionalidad del sistema en general</t>
+  </si>
+  <si>
+    <t>Riesgos de Terceros</t>
+  </si>
+  <si>
+    <t>Dependencia excesiva de proveedores externos o socios estratégicos puede exponer al proyecto a riesgos relacionados con la calidad, disponibilidad o confiabilidad de los servicios proporcionados por estos terceros</t>
+  </si>
+  <si>
+    <t>Desafíos de Capacitación del Usuario Final</t>
+  </si>
+  <si>
+    <t>La implementación de nuevas funcionalidades puede requerir una capacitación adecuada para los usuarios finales. La falta de una estrategia de capacitación efectiva puede resultar en una adopción deficiente de las nuevas funcionalidades y afectar la eficacia del proyecto</t>
+  </si>
+  <si>
+    <t>Problemas de Gestión de Alcance</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> La falta de una gestión efectiva del alcance del proyecto puede llevar a la inclusión de funcionalidades adicionales no planificadas inicialmente, lo que podría resultar en retrasos y aumento de costos</t>
+  </si>
+  <si>
+    <t>Riesgos de Cumplimiento Normativo</t>
+  </si>
+  <si>
+    <t>Los cambios en las regulaciones y normativas gubernamentales pueden afectar la implementación de nuevas funcionalidades. La falta de cumplimiento normativo puede resultar en multas, sanciones legales y daños a la reputación de la empresa. Es importante monitorear de cerca cualquier cambio en el entorno regulatorio y asegurarse de que el proyecto esté alineado con todas las leyes y regulaciones pertinentes</t>
+  </si>
+  <si>
+    <t>R30</t>
+  </si>
+  <si>
+    <t>Riesgos de Disponibilidad de Recursos Tecnológicos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> La falta de acceso a recursos tecnológicos adecuados, como servidores, infraestructura de red o herramientas de desarrollo, puede obstaculizar la implementación efectiva de nuevas funcionalidades. Esto podría conducir a retrasos en el proyecto, interrupciones en el desarrollo y dificultades para mantener la calidad del producto final. Es esencial contar con un plan sólido para garantizar la disponibilidad y el acceso a los recursos tecnológicos necesarios durante todo el ciclo de vida del proyecto</t>
+  </si>
+  <si>
+    <t>Fortalecimiento de los sistemas de seguridad, auditorías regulares, cifrado de datos sensibles, capacitación del personal en seguridad, respuesta rápida ante incidentes y comunicación transparente con los clientes en caso de brechas</t>
+  </si>
+  <si>
+    <t>Monitorización activa de tendencias de mercado, la diversificación del catálogo de productos, la inversión en investigación y desarrollo para adaptar los productos a las nuevas demandas, y una comunicación efectiva con los clientes para comprender y satisfacer sus necesidades en evolución</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> se implementarían medidas tales como la revisión y actualización periódica de las descripciones de productos, la verificación cruzada de la información proporcionada por múltiples fuentes, la capacitación del personal en la creación de descripciones precisas y detalladas, y la recopilación activa de comentarios de los clientes para identificar y corregir cualquier discrepancia o falta de información</t>
+  </si>
+  <si>
+    <t>se implementarían estrategias como la verificación regular de la calidad de las imágenes, la optimización de la velocidad de carga de las mismas, la colaboración con proveedores confiables para obtener imágenes de alta calidad, y la implementación de herramientas que permitan a los clientes ver el producto desde diferentes ángulos o en diferentes contextos para una mejor visualización</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> la sincronización precisa entre el sistema de gestión de inventario y la plataforma de venta en línea, y la comunicación proactiva con los clientes sobre el estado del stock y las opciones de reabastecimiento, garantizando así una experiencia satisfactoria para los clientes y evitando posibles inconvenientes por productos no disponibles</t>
+  </si>
+  <si>
+    <t>se realizarían pruebas de usabilidad, se corregirían enlaces rotos rápidamente y se diseñarían interfaces intuitivas, asegurando una experiencia fluida para los clientes y disminuyendo la posibilidad de que opten por comprar en otros lugares.</t>
+  </si>
+  <si>
+    <t>se realizarían pruebas exhaustivas, se corregirían rápidamente los errores y se simplificaría el proceso de compra</t>
+  </si>
+  <si>
+    <t>revisiones regulares, empleo de traductores profesionales y herramientas de localización eficaces para garantizar una experiencia óptima para clientes de diferentes idiomas</t>
+  </si>
+  <si>
+    <t>Se solucionaría mediante revisión continua, uso de algoritmos mejorados y retroalimentación de los clientes para mejorar la precisión de la categorización y la relevancia de las recomendaciones</t>
+  </si>
+  <si>
+    <t>se incentivaría activamente la retroalimentación de los clientes, se ofrecerían incentivos para dejar reseñas y se destacarían las reseñas existentes para aumentar la confianza en la calidad del producto</t>
+  </si>
+  <si>
+    <t>Se resolvería optimizando la velocidad del sitio mediante técnicas de optimización de rendimiento, como la compresión de archivos, el almacenamiento en caché y la optimización de imágenes, para garantizar una experiencia de usuario rápida y fluida</t>
+  </si>
+  <si>
+    <t>Se abordaría mediante una planificación cuidadosa, asignación adecuada de recursos y seguimiento regular del progreso para garantizar el cumplimiento de los plazos y mantener la competitividad en el mercado</t>
+  </si>
+  <si>
+    <t>Se corregiría con una planificación exhaustiva, identificación anticipada de posibles obstáculos y ajustes en el plan según sea necesario para mantener el proyecto dentro del presupuesto y los plazos establecidos</t>
+  </si>
+  <si>
+    <t>Se manejaría anticipándolos, manteniendo flexibilidad en la arquitectura y actualizándose constantemente sobre avances tecnológicos para minimizar el impacto en el proyecto</t>
+  </si>
+  <si>
+    <t>Se resolvería mediante una planificación detallada de integración, pruebas exhaustivas y colaboración estrecha entre equipos para garantizar una implementación sin problemas de nuevas funcionalidades</t>
+  </si>
+  <si>
+    <t>e manejaría diversificando proveedores, estableciendo acuerdos claros y realizando un seguimiento cercano para mitigar cualquier impacto negativo en el proyecto</t>
+  </si>
+  <si>
+    <t>Se resolvería mediante la implementación de una estrategia de capacitación sólida, que incluya materiales claros y accesibles, sesiones prácticas y soporte continuo para garantizar una adopción exitosa y la eficacia del proyecto</t>
+  </si>
+  <si>
+    <t>Se manejarían mediante una definición clara del alcance inicial, comunicación constante con los interesados y un proceso establecido para gestionar y controlar cualquier cambio en el alcance del proyecto</t>
+  </si>
+  <si>
+    <t>Se abordarían mediante un monitoreo constante del entorno regulatorio, asegurando la alineación del proyecto con las leyes y regulaciones pertinentes, y ajustando el enfoque del proyecto según sea necesario para garantizar el cumplimiento y evitar posibles sanciones legales y daños a la reputación</t>
+  </si>
+  <si>
+    <t>Se abordaría mediante la planificación anticipada de necesidades de recursos, la identificación de proveedores confiables y la implementación de un plan de contingencia para garantizar la disponibilidad y el acceso a los recursos necesarios en todas las etapas del proyecto</t>
+  </si>
+  <si>
+    <t>CBA: 5</t>
+  </si>
+  <si>
+    <t>CBA: 6</t>
+  </si>
+  <si>
+    <t>CBA: 7</t>
+  </si>
+  <si>
+    <t>CBA: 8</t>
+  </si>
+  <si>
+    <t>CBA: 9</t>
+  </si>
+  <si>
+    <t>CBA: 10</t>
+  </si>
+  <si>
+    <t>CBA: 11</t>
+  </si>
+  <si>
+    <t>CBA: 12</t>
+  </si>
+  <si>
+    <t>CBA: 13</t>
+  </si>
+  <si>
+    <t>CBA: 14</t>
+  </si>
+  <si>
+    <t>CBA: 15</t>
+  </si>
+  <si>
+    <t>CBA: 16</t>
+  </si>
+  <si>
+    <t>CBA: 17</t>
+  </si>
+  <si>
+    <t>CBA: 18</t>
+  </si>
+  <si>
+    <t>CBA: 19</t>
+  </si>
+  <si>
+    <t>CBA: 20</t>
+  </si>
+  <si>
+    <t>CBA: 21</t>
+  </si>
+  <si>
+    <t>CBA: 22</t>
+  </si>
+  <si>
+    <t>CBA: 23</t>
   </si>
 </sst>
 </file>
@@ -1111,8 +1336,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AV303"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="72" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="72" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -1155,7 +1380,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:48" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:48" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
@@ -1166,7 +1391,7 @@
         <v>19</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>17</v>
@@ -1178,30 +1403,27 @@
         <v>20</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="L2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="L2" s="21" t="s">
         <v>10</v>
       </c>
+      <c r="M2" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="N2" s="7" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="P2" s="7" t="s">
         <v>3</v>
       </c>
       <c r="Y2" s="33">
@@ -1220,7 +1442,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:48" s="13" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:48" s="13" customFormat="1" ht="82.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>29</v>
       </c>
@@ -1231,7 +1453,7 @@
         <v>45362</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>34</v>
@@ -1243,29 +1465,26 @@
         <v>36</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="I3" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="K3" s="11"/>
-      <c r="L3" s="5">
+      <c r="J3" s="11"/>
+      <c r="K3" s="5">
         <v>3</v>
       </c>
-      <c r="M3" s="34">
+      <c r="L3" s="34">
         <v>1</v>
       </c>
-      <c r="N3" s="5">
-        <f>L3*M3</f>
+      <c r="M3" s="5">
+        <f>K3*L3</f>
         <v>3</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="N3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="P3" s="11"/>
+      <c r="O3" s="11"/>
       <c r="Q3" s="12"/>
       <c r="R3" s="12"/>
       <c r="S3" s="12"/>
@@ -1299,7 +1518,7 @@
       <c r="AU3" s="12"/>
       <c r="AV3" s="12"/>
     </row>
-    <row r="4" spans="1:48" ht="96" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:48" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>31</v>
       </c>
@@ -1310,7 +1529,7 @@
         <v>45363</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>47</v>
@@ -1322,29 +1541,26 @@
         <v>35</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="I4" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="K4" s="11"/>
-      <c r="L4" s="5">
+      <c r="J4" s="11"/>
+      <c r="K4" s="5">
         <v>5</v>
       </c>
-      <c r="M4" s="34">
+      <c r="L4" s="34">
         <v>2</v>
       </c>
-      <c r="N4" s="5">
-        <f>L4*M4</f>
+      <c r="M4" s="5">
+        <f>K4*L4</f>
         <v>10</v>
       </c>
-      <c r="O4" s="10" t="s">
+      <c r="N4" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="P4" s="11"/>
+      <c r="O4" s="11"/>
     </row>
     <row r="5" spans="1:48" ht="66" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
@@ -1357,7 +1573,7 @@
         <v>45364</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>37</v>
@@ -1369,31 +1585,28 @@
         <v>38</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="J5" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="I5" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="K5" s="11"/>
-      <c r="L5" s="5">
+      <c r="J5" s="11"/>
+      <c r="K5" s="5">
         <v>5</v>
       </c>
-      <c r="M5" s="34">
+      <c r="L5" s="34">
         <v>1</v>
       </c>
-      <c r="N5" s="5">
-        <f>L5*M5</f>
+      <c r="M5" s="5">
+        <f>K5*L5</f>
         <v>5</v>
       </c>
-      <c r="O5" s="10" t="s">
+      <c r="N5" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="P5" s="11"/>
-    </row>
-    <row r="6" spans="1:48" ht="66" x14ac:dyDescent="0.3">
+      <c r="O5" s="11"/>
+    </row>
+    <row r="6" spans="1:48" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>33</v>
       </c>
@@ -1404,10 +1617,10 @@
         <v>45365</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>43</v>
@@ -1416,31 +1629,28 @@
         <v>46</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="J6" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="I6" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="K6" s="11"/>
-      <c r="L6" s="5">
+      <c r="J6" s="11"/>
+      <c r="K6" s="5">
         <v>5</v>
       </c>
-      <c r="M6" s="34">
+      <c r="L6" s="34">
         <v>1</v>
       </c>
-      <c r="N6" s="5">
-        <f t="shared" ref="N6" si="0">L6*M6</f>
+      <c r="M6" s="5">
+        <f t="shared" ref="M6" si="0">K6*L6</f>
         <v>5</v>
       </c>
-      <c r="O6" s="10" t="s">
+      <c r="N6" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="P6" s="11"/>
-    </row>
-    <row r="7" spans="1:48" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="O6" s="11"/>
+    </row>
+    <row r="7" spans="1:48" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>39</v>
       </c>
@@ -1451,10 +1661,10 @@
         <v>45366</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>44</v>
@@ -1463,29 +1673,26 @@
         <v>48</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="J7" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="I7" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="K7" s="11"/>
-      <c r="L7" s="5">
+      <c r="J7" s="11"/>
+      <c r="K7" s="5">
         <v>4</v>
       </c>
-      <c r="M7" s="34">
+      <c r="L7" s="34">
         <v>1</v>
       </c>
-      <c r="N7" s="5">
-        <f t="shared" ref="N7:N12" si="1">L7*M7</f>
+      <c r="M7" s="5">
+        <f t="shared" ref="M7:M12" si="1">K7*L7</f>
         <v>4</v>
       </c>
-      <c r="O7" s="10" t="s">
+      <c r="N7" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="P7" s="11"/>
+      <c r="O7" s="11"/>
     </row>
     <row r="8" spans="1:48" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
@@ -1498,10 +1705,10 @@
         <v>45367</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>57</v>
@@ -1510,31 +1717,28 @@
         <v>58</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="K8" s="6"/>
-      <c r="L8" s="5">
+        <v>87</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8" s="6"/>
+      <c r="K8" s="5">
         <v>4</v>
       </c>
-      <c r="M8" s="34">
+      <c r="L8" s="34">
         <v>4</v>
       </c>
-      <c r="N8" s="5">
+      <c r="M8" s="5">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="O8" s="10" t="s">
+      <c r="N8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="P8" s="6"/>
-    </row>
-    <row r="9" spans="1:48" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="O8" s="6"/>
+    </row>
+    <row r="9" spans="1:48" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>53</v>
       </c>
@@ -1545,41 +1749,38 @@
         <v>45368</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F9" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="G9" s="8" t="s">
-        <v>61</v>
-      </c>
       <c r="H9" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="K9" s="6"/>
-      <c r="L9" s="5">
+        <v>87</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="J9" s="6"/>
+      <c r="K9" s="5">
         <v>4</v>
       </c>
-      <c r="M9" s="34">
+      <c r="L9" s="34">
         <v>3</v>
       </c>
-      <c r="N9" s="5">
+      <c r="M9" s="5">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="O9" s="10" t="s">
+      <c r="N9" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="P9" s="6"/>
+      <c r="O9" s="6"/>
     </row>
     <row r="10" spans="1:48" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
@@ -1592,43 +1793,40 @@
         <v>45369</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="K10" s="6"/>
-      <c r="L10" s="5">
+        <v>87</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="J10" s="6"/>
+      <c r="K10" s="5">
         <v>3</v>
       </c>
-      <c r="M10" s="34">
+      <c r="L10" s="34">
         <v>2</v>
       </c>
-      <c r="N10" s="5">
-        <f>L10*M10</f>
+      <c r="M10" s="5">
+        <f>K10*L10</f>
         <v>6</v>
       </c>
-      <c r="O10" s="10" t="s">
+      <c r="N10" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="P10" s="6"/>
-    </row>
-    <row r="11" spans="1:48" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="O10" s="6"/>
+    </row>
+    <row r="11" spans="1:48" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>55</v>
       </c>
@@ -1639,41 +1837,38 @@
         <v>45370</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F11" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="8" t="s">
-        <v>64</v>
-      </c>
       <c r="H11" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="J11" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="K11" s="6"/>
-      <c r="L11" s="5">
+        <v>87</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="J11" s="6"/>
+      <c r="K11" s="5">
         <v>4</v>
       </c>
-      <c r="M11" s="34">
+      <c r="L11" s="34">
         <v>3</v>
       </c>
-      <c r="N11" s="5">
+      <c r="M11" s="5">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="O11" s="10" t="s">
+      <c r="N11" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="P11" s="6"/>
+      <c r="O11" s="6"/>
     </row>
     <row r="12" spans="1:48" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
@@ -1686,45 +1881,42 @@
         <v>45371</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>121</v>
+        <v>138</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F12" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="G12" s="10" t="s">
-        <v>74</v>
-      </c>
       <c r="H12" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J12" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="K12" s="11"/>
-      <c r="L12" s="5">
+        <v>45</v>
+      </c>
+      <c r="J12" s="11"/>
+      <c r="K12" s="5">
         <v>3</v>
       </c>
-      <c r="M12" s="34">
+      <c r="L12" s="34">
         <v>4</v>
       </c>
-      <c r="N12" s="5">
+      <c r="M12" s="5">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="O12" s="10" t="s">
+      <c r="N12" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="P12" s="9"/>
-    </row>
-    <row r="13" spans="1:48" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O12" s="9"/>
+    </row>
+    <row r="13" spans="1:48" ht="133.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>51</v>
@@ -1733,41 +1925,38 @@
         <v>45372</v>
       </c>
       <c r="D13" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="E13" s="10" t="s">
-        <v>109</v>
-      </c>
       <c r="F13" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>74</v>
+        <v>158</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J13" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="K13" s="11"/>
-      <c r="L13" s="5">
-        <v>3</v>
-      </c>
-      <c r="M13" s="34">
-        <v>4</v>
-      </c>
-      <c r="N13" s="5">
-        <f t="shared" ref="N13:N26" si="2">L13*M13</f>
-        <v>12</v>
-      </c>
-      <c r="O13" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="J13" s="11"/>
+      <c r="K13" s="5">
+        <v>5</v>
+      </c>
+      <c r="L13" s="34">
+        <v>2</v>
+      </c>
+      <c r="M13" s="5">
+        <f t="shared" ref="M13:M26" si="2">K13*L13</f>
+        <v>10</v>
+      </c>
+      <c r="N13" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="P13" s="9"/>
+      <c r="O13" s="9"/>
       <c r="AI13" s="1"/>
       <c r="AJ13" s="1"/>
       <c r="AK13" s="1"/>
@@ -1783,9 +1972,9 @@
       <c r="AU13" s="1"/>
       <c r="AV13" s="1"/>
     </row>
-    <row r="14" spans="1:48" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:48" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>51</v>
@@ -1794,41 +1983,38 @@
         <v>45373</v>
       </c>
       <c r="D14" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="E14" s="10" t="s">
-        <v>111</v>
-      </c>
       <c r="F14" s="8" t="s">
-        <v>73</v>
+        <v>178</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>74</v>
+        <v>159</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J14" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="K14" s="11"/>
-      <c r="L14" s="5">
-        <v>3</v>
-      </c>
-      <c r="M14" s="34">
+        <v>45</v>
+      </c>
+      <c r="J14" s="11"/>
+      <c r="K14" s="5">
+        <v>1</v>
+      </c>
+      <c r="L14" s="34">
         <v>4</v>
       </c>
-      <c r="N14" s="5">
+      <c r="M14" s="5">
         <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="O14" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="N14" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="P14" s="9"/>
+      <c r="O14" s="9"/>
       <c r="AI14" s="1"/>
       <c r="AJ14" s="1"/>
       <c r="AK14" s="1"/>
@@ -1844,9 +2030,9 @@
       <c r="AU14" s="1"/>
       <c r="AV14" s="1"/>
     </row>
-    <row r="15" spans="1:48" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:48" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>51</v>
@@ -1854,40 +2040,39 @@
       <c r="C15" s="6">
         <v>45374</v>
       </c>
-      <c r="D15" s="10"/>
+      <c r="D15" s="10" t="s">
+        <v>117</v>
+      </c>
       <c r="E15" s="10" t="s">
-        <v>83</v>
+        <v>118</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>73</v>
+        <v>179</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>74</v>
+        <v>160</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J15" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="K15" s="11"/>
-      <c r="L15" s="5">
+        <v>45</v>
+      </c>
+      <c r="J15" s="11"/>
+      <c r="K15" s="5">
+        <v>1</v>
+      </c>
+      <c r="L15" s="34">
         <v>3</v>
       </c>
-      <c r="M15" s="34">
-        <v>4</v>
-      </c>
-      <c r="N15" s="5">
+      <c r="M15" s="5">
         <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="O15" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="N15" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="P15" s="9"/>
+      <c r="O15" s="9"/>
       <c r="AI15" s="1"/>
       <c r="AJ15" s="1"/>
       <c r="AK15" s="1"/>
@@ -1903,9 +2088,9 @@
       <c r="AU15" s="1"/>
       <c r="AV15" s="1"/>
     </row>
-    <row r="16" spans="1:48" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:48" ht="120.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>51</v>
@@ -1913,40 +2098,39 @@
       <c r="C16" s="6">
         <v>45375</v>
       </c>
-      <c r="D16" s="10"/>
+      <c r="D16" s="10" t="s">
+        <v>119</v>
+      </c>
       <c r="E16" s="10" t="s">
-        <v>83</v>
+        <v>126</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>73</v>
+        <v>180</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>74</v>
+        <v>161</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J16" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="K16" s="11"/>
-      <c r="L16" s="5">
-        <v>3</v>
-      </c>
-      <c r="M16" s="34">
+        <v>45</v>
+      </c>
+      <c r="J16" s="11"/>
+      <c r="K16" s="5">
+        <v>1</v>
+      </c>
+      <c r="L16" s="34">
         <v>4</v>
       </c>
-      <c r="N16" s="5">
+      <c r="M16" s="5">
         <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="O16" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="N16" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="P16" s="9"/>
+      <c r="O16" s="9"/>
       <c r="AI16" s="1"/>
       <c r="AJ16" s="1"/>
       <c r="AK16" s="1"/>
@@ -1962,9 +2146,9 @@
       <c r="AU16" s="1"/>
       <c r="AV16" s="1"/>
     </row>
-    <row r="17" spans="1:48" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:48" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>51</v>
@@ -1972,40 +2156,39 @@
       <c r="C17" s="6">
         <v>45376</v>
       </c>
-      <c r="D17" s="10"/>
+      <c r="D17" s="10" t="s">
+        <v>120</v>
+      </c>
       <c r="E17" s="10" t="s">
-        <v>83</v>
+        <v>121</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>73</v>
+        <v>181</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>74</v>
+        <v>162</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J17" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="K17" s="11"/>
-      <c r="L17" s="5">
+        <v>45</v>
+      </c>
+      <c r="J17" s="11"/>
+      <c r="K17" s="5">
         <v>3</v>
       </c>
-      <c r="M17" s="34">
-        <v>4</v>
-      </c>
-      <c r="N17" s="5">
+      <c r="L17" s="34">
+        <v>3</v>
+      </c>
+      <c r="M17" s="5">
         <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="O17" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="N17" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="P17" s="9"/>
+      <c r="O17" s="9"/>
       <c r="AI17" s="1"/>
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1"/>
@@ -2021,9 +2204,9 @@
       <c r="AU17" s="1"/>
       <c r="AV17" s="1"/>
     </row>
-    <row r="18" spans="1:48" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:48" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>51</v>
@@ -2031,40 +2214,39 @@
       <c r="C18" s="6">
         <v>45377</v>
       </c>
-      <c r="D18" s="10"/>
+      <c r="D18" s="10" t="s">
+        <v>122</v>
+      </c>
       <c r="E18" s="10" t="s">
-        <v>83</v>
+        <v>123</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>73</v>
+        <v>182</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>74</v>
+        <v>163</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J18" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="K18" s="11"/>
-      <c r="L18" s="5">
+        <v>45</v>
+      </c>
+      <c r="J18" s="11"/>
+      <c r="K18" s="5">
         <v>3</v>
       </c>
-      <c r="M18" s="34">
-        <v>4</v>
-      </c>
-      <c r="N18" s="5">
+      <c r="L18" s="34">
+        <v>3</v>
+      </c>
+      <c r="M18" s="5">
         <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="O18" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="N18" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="P18" s="9"/>
+      <c r="O18" s="9"/>
       <c r="AI18" s="1"/>
       <c r="AJ18" s="1"/>
       <c r="AK18" s="1"/>
@@ -2080,9 +2262,9 @@
       <c r="AU18" s="1"/>
       <c r="AV18" s="1"/>
     </row>
-    <row r="19" spans="1:48" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:48" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>51</v>
@@ -2090,40 +2272,39 @@
       <c r="C19" s="6">
         <v>45378</v>
       </c>
-      <c r="D19" s="10"/>
+      <c r="D19" s="10" t="s">
+        <v>124</v>
+      </c>
       <c r="E19" s="10" t="s">
-        <v>83</v>
+        <v>125</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>73</v>
+        <v>183</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>74</v>
+        <v>164</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J19" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="K19" s="11"/>
-      <c r="L19" s="5">
-        <v>3</v>
-      </c>
-      <c r="M19" s="34">
-        <v>4</v>
-      </c>
-      <c r="N19" s="5">
+        <v>45</v>
+      </c>
+      <c r="J19" s="11"/>
+      <c r="K19" s="5">
+        <v>5</v>
+      </c>
+      <c r="L19" s="34">
+        <v>2</v>
+      </c>
+      <c r="M19" s="5">
         <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="O19" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="N19" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="P19" s="9"/>
+      <c r="O19" s="9"/>
       <c r="AI19" s="1"/>
       <c r="AJ19" s="1"/>
       <c r="AK19" s="1"/>
@@ -2139,9 +2320,9 @@
       <c r="AU19" s="1"/>
       <c r="AV19" s="1"/>
     </row>
-    <row r="20" spans="1:48" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:48" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>51</v>
@@ -2149,40 +2330,39 @@
       <c r="C20" s="6">
         <v>45379</v>
       </c>
-      <c r="D20" s="10"/>
+      <c r="D20" s="10" t="s">
+        <v>127</v>
+      </c>
       <c r="E20" s="10" t="s">
-        <v>83</v>
+        <v>128</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>73</v>
+        <v>184</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>74</v>
+        <v>165</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J20" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="K20" s="11"/>
-      <c r="L20" s="5">
-        <v>3</v>
-      </c>
-      <c r="M20" s="34">
+        <v>45</v>
+      </c>
+      <c r="J20" s="11"/>
+      <c r="K20" s="5">
         <v>4</v>
       </c>
-      <c r="N20" s="5">
+      <c r="L20" s="34">
+        <v>2</v>
+      </c>
+      <c r="M20" s="5">
         <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="O20" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="N20" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="P20" s="9"/>
+      <c r="O20" s="9"/>
       <c r="AI20" s="1"/>
       <c r="AJ20" s="1"/>
       <c r="AK20" s="1"/>
@@ -2198,9 +2378,9 @@
       <c r="AU20" s="1"/>
       <c r="AV20" s="1"/>
     </row>
-    <row r="21" spans="1:48" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:48" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>51</v>
@@ -2208,40 +2388,39 @@
       <c r="C21" s="6">
         <v>45380</v>
       </c>
-      <c r="D21" s="10"/>
+      <c r="D21" s="10" t="s">
+        <v>129</v>
+      </c>
       <c r="E21" s="10" t="s">
-        <v>83</v>
+        <v>130</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>73</v>
+        <v>185</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>74</v>
+        <v>166</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J21" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="K21" s="11"/>
-      <c r="L21" s="5">
+        <v>45</v>
+      </c>
+      <c r="J21" s="11"/>
+      <c r="K21" s="5">
         <v>3</v>
       </c>
-      <c r="M21" s="34">
-        <v>4</v>
-      </c>
-      <c r="N21" s="5">
+      <c r="L21" s="34">
+        <v>2</v>
+      </c>
+      <c r="M21" s="5">
         <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="O21" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="N21" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="P21" s="9"/>
+      <c r="O21" s="9"/>
       <c r="AI21" s="1"/>
       <c r="AJ21" s="1"/>
       <c r="AK21" s="1"/>
@@ -2257,50 +2436,49 @@
       <c r="AU21" s="1"/>
       <c r="AV21" s="1"/>
     </row>
-    <row r="22" spans="1:48" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:48" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C22" s="6">
         <v>45381</v>
       </c>
-      <c r="D22" s="10"/>
+      <c r="D22" s="10" t="s">
+        <v>131</v>
+      </c>
       <c r="E22" s="10" t="s">
-        <v>83</v>
+        <v>132</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>73</v>
+        <v>186</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>74</v>
+        <v>167</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J22" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="K22" s="11"/>
-      <c r="L22" s="5">
-        <v>3</v>
-      </c>
-      <c r="M22" s="34">
-        <v>4</v>
-      </c>
-      <c r="N22" s="5">
+        <v>45</v>
+      </c>
+      <c r="J22" s="11"/>
+      <c r="K22" s="5">
+        <v>1</v>
+      </c>
+      <c r="L22" s="34">
+        <v>5</v>
+      </c>
+      <c r="M22" s="5">
         <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="O22" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="N22" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="P22" s="9"/>
+      <c r="O22" s="9"/>
       <c r="AI22" s="1"/>
       <c r="AJ22" s="1"/>
       <c r="AK22" s="1"/>
@@ -2316,50 +2494,49 @@
       <c r="AU22" s="1"/>
       <c r="AV22" s="1"/>
     </row>
-    <row r="23" spans="1:48" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:48" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C23" s="6">
         <v>45382</v>
       </c>
-      <c r="D23" s="10"/>
+      <c r="D23" s="10" t="s">
+        <v>133</v>
+      </c>
       <c r="E23" s="10" t="s">
-        <v>83</v>
+        <v>134</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>73</v>
+        <v>187</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>74</v>
+        <v>168</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J23" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="K23" s="11"/>
-      <c r="L23" s="5">
-        <v>3</v>
-      </c>
-      <c r="M23" s="34">
-        <v>4</v>
-      </c>
-      <c r="N23" s="5">
+        <v>45</v>
+      </c>
+      <c r="J23" s="11"/>
+      <c r="K23" s="5">
+        <v>5</v>
+      </c>
+      <c r="L23" s="34">
+        <v>1</v>
+      </c>
+      <c r="M23" s="5">
         <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="O23" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="N23" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="P23" s="9"/>
+      <c r="O23" s="9"/>
       <c r="AI23" s="1"/>
       <c r="AJ23" s="1"/>
       <c r="AK23" s="1"/>
@@ -2375,9 +2552,9 @@
       <c r="AU23" s="1"/>
       <c r="AV23" s="1"/>
     </row>
-    <row r="24" spans="1:48" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:48" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>50</v>
@@ -2385,40 +2562,39 @@
       <c r="C24" s="6">
         <v>45383</v>
       </c>
-      <c r="D24" s="10"/>
+      <c r="D24" s="10" t="s">
+        <v>139</v>
+      </c>
       <c r="E24" s="10" t="s">
-        <v>83</v>
+        <v>140</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>73</v>
+        <v>188</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>74</v>
+        <v>169</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J24" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="K24" s="11"/>
-      <c r="L24" s="5">
+        <v>45</v>
+      </c>
+      <c r="J24" s="11"/>
+      <c r="K24" s="5">
+        <v>5</v>
+      </c>
+      <c r="L24" s="34">
         <v>3</v>
       </c>
-      <c r="M24" s="34">
-        <v>4</v>
-      </c>
-      <c r="N24" s="5">
+      <c r="M24" s="5">
         <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="O24" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="N24" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="P24" s="9"/>
+      <c r="O24" s="9"/>
       <c r="AI24" s="1"/>
       <c r="AJ24" s="1"/>
       <c r="AK24" s="1"/>
@@ -2434,9 +2610,9 @@
       <c r="AU24" s="1"/>
       <c r="AV24" s="1"/>
     </row>
-    <row r="25" spans="1:48" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:48" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>50</v>
@@ -2444,40 +2620,39 @@
       <c r="C25" s="6">
         <v>45384</v>
       </c>
-      <c r="D25" s="10"/>
+      <c r="D25" s="10" t="s">
+        <v>141</v>
+      </c>
       <c r="E25" s="10" t="s">
-        <v>83</v>
+        <v>142</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>73</v>
+        <v>189</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>74</v>
+        <v>170</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J25" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="K25" s="11"/>
-      <c r="L25" s="5">
+        <v>45</v>
+      </c>
+      <c r="J25" s="11"/>
+      <c r="K25" s="5">
+        <v>4</v>
+      </c>
+      <c r="L25" s="34">
         <v>3</v>
       </c>
-      <c r="M25" s="34">
-        <v>4</v>
-      </c>
-      <c r="N25" s="5">
+      <c r="M25" s="5">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="O25" s="10" t="s">
+      <c r="N25" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="P25" s="9"/>
+      <c r="O25" s="9"/>
       <c r="AI25" s="1"/>
       <c r="AJ25" s="1"/>
       <c r="AK25" s="1"/>
@@ -2493,9 +2668,9 @@
       <c r="AU25" s="1"/>
       <c r="AV25" s="1"/>
     </row>
-    <row r="26" spans="1:48" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:48" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>50</v>
@@ -2503,40 +2678,39 @@
       <c r="C26" s="6">
         <v>45385</v>
       </c>
-      <c r="D26" s="10"/>
+      <c r="D26" s="10" t="s">
+        <v>143</v>
+      </c>
       <c r="E26" s="10" t="s">
-        <v>83</v>
+        <v>144</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>73</v>
+        <v>190</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>74</v>
+        <v>171</v>
       </c>
       <c r="H26" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J26" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="K26" s="11"/>
-      <c r="L26" s="5">
+        <v>45</v>
+      </c>
+      <c r="J26" s="11"/>
+      <c r="K26" s="5">
         <v>3</v>
       </c>
-      <c r="M26" s="34">
+      <c r="L26" s="34">
         <v>4</v>
       </c>
-      <c r="N26" s="5">
+      <c r="M26" s="5">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="O26" s="10" t="s">
+      <c r="N26" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="P26" s="9"/>
+      <c r="O26" s="9"/>
       <c r="AI26" s="1"/>
       <c r="AJ26" s="1"/>
       <c r="AK26" s="1"/>
@@ -2552,9 +2726,9 @@
       <c r="AU26" s="1"/>
       <c r="AV26" s="1"/>
     </row>
-    <row r="27" spans="1:48" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:48" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>50</v>
@@ -2562,40 +2736,39 @@
       <c r="C27" s="6">
         <v>45386</v>
       </c>
-      <c r="D27" s="10"/>
+      <c r="D27" s="10" t="s">
+        <v>145</v>
+      </c>
       <c r="E27" s="10" t="s">
-        <v>83</v>
+        <v>146</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>73</v>
+        <v>191</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>74</v>
+        <v>172</v>
       </c>
       <c r="H27" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I27" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J27" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="K27" s="11"/>
-      <c r="L27" s="5">
-        <v>3</v>
-      </c>
-      <c r="M27" s="34">
+        <v>45</v>
+      </c>
+      <c r="J27" s="11"/>
+      <c r="K27" s="5">
         <v>4</v>
       </c>
-      <c r="N27" s="5">
-        <f t="shared" ref="N27:N31" si="3">L27*M27</f>
-        <v>12</v>
-      </c>
-      <c r="O27" s="10" t="s">
+      <c r="L27" s="34">
+        <v>2</v>
+      </c>
+      <c r="M27" s="5">
+        <f t="shared" ref="M27:M31" si="3">K27*L27</f>
+        <v>8</v>
+      </c>
+      <c r="N27" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="P27" s="9"/>
+      <c r="O27" s="9"/>
       <c r="AI27" s="1"/>
       <c r="AJ27" s="1"/>
       <c r="AK27" s="1"/>
@@ -2611,9 +2784,9 @@
       <c r="AU27" s="1"/>
       <c r="AV27" s="1"/>
     </row>
-    <row r="28" spans="1:48" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:48" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>50</v>
@@ -2621,40 +2794,39 @@
       <c r="C28" s="6">
         <v>45387</v>
       </c>
-      <c r="D28" s="10"/>
+      <c r="D28" s="10" t="s">
+        <v>147</v>
+      </c>
       <c r="E28" s="10" t="s">
-        <v>83</v>
+        <v>148</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>73</v>
+        <v>192</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>74</v>
+        <v>173</v>
       </c>
       <c r="H28" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J28" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="K28" s="11"/>
-      <c r="L28" s="5">
+        <v>45</v>
+      </c>
+      <c r="J28" s="11"/>
+      <c r="K28" s="5">
         <v>3</v>
       </c>
-      <c r="M28" s="34">
-        <v>4</v>
-      </c>
-      <c r="N28" s="5">
+      <c r="L28" s="34">
+        <v>2</v>
+      </c>
+      <c r="M28" s="5">
         <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="O28" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="N28" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="P28" s="9"/>
+      <c r="O28" s="9"/>
       <c r="AI28" s="1"/>
       <c r="AJ28" s="1"/>
       <c r="AK28" s="1"/>
@@ -2670,9 +2842,9 @@
       <c r="AU28" s="1"/>
       <c r="AV28" s="1"/>
     </row>
-    <row r="29" spans="1:48" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:48" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>50</v>
@@ -2680,40 +2852,39 @@
       <c r="C29" s="6">
         <v>45388</v>
       </c>
-      <c r="D29" s="10"/>
+      <c r="D29" s="10" t="s">
+        <v>149</v>
+      </c>
       <c r="E29" s="10" t="s">
-        <v>83</v>
+        <v>150</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>73</v>
+        <v>193</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>74</v>
+        <v>174</v>
       </c>
       <c r="H29" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I29" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J29" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="K29" s="11"/>
-      <c r="L29" s="5">
+        <v>45</v>
+      </c>
+      <c r="J29" s="11"/>
+      <c r="K29" s="5">
         <v>3</v>
       </c>
-      <c r="M29" s="34">
+      <c r="L29" s="34">
         <v>4</v>
       </c>
-      <c r="N29" s="5">
+      <c r="M29" s="5">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="O29" s="10" t="s">
+      <c r="N29" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="P29" s="9"/>
+      <c r="O29" s="9"/>
       <c r="AI29" s="1"/>
       <c r="AJ29" s="1"/>
       <c r="AK29" s="1"/>
@@ -2729,9 +2900,9 @@
       <c r="AU29" s="1"/>
       <c r="AV29" s="1"/>
     </row>
-    <row r="30" spans="1:48" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:48" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>50</v>
@@ -2739,40 +2910,39 @@
       <c r="C30" s="6">
         <v>45389</v>
       </c>
-      <c r="D30" s="10"/>
+      <c r="D30" s="10" t="s">
+        <v>151</v>
+      </c>
       <c r="E30" s="10" t="s">
-        <v>83</v>
+        <v>152</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>73</v>
+        <v>194</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>74</v>
+        <v>175</v>
       </c>
       <c r="H30" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I30" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J30" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="K30" s="11"/>
-      <c r="L30" s="5">
-        <v>3</v>
-      </c>
-      <c r="M30" s="34">
+        <v>45</v>
+      </c>
+      <c r="J30" s="11"/>
+      <c r="K30" s="5">
+        <v>2</v>
+      </c>
+      <c r="L30" s="34">
         <v>4</v>
       </c>
-      <c r="N30" s="5">
+      <c r="M30" s="5">
         <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="O30" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="N30" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="P30" s="9"/>
+      <c r="O30" s="9"/>
       <c r="AI30" s="1"/>
       <c r="AJ30" s="1"/>
       <c r="AK30" s="1"/>
@@ -2788,9 +2958,9 @@
       <c r="AU30" s="1"/>
       <c r="AV30" s="1"/>
     </row>
-    <row r="31" spans="1:48" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:48" ht="129.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>50</v>
@@ -2798,40 +2968,39 @@
       <c r="C31" s="6">
         <v>45390</v>
       </c>
-      <c r="D31" s="10"/>
+      <c r="D31" s="10" t="s">
+        <v>153</v>
+      </c>
       <c r="E31" s="10" t="s">
-        <v>83</v>
+        <v>154</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>73</v>
+        <v>195</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>74</v>
+        <v>176</v>
       </c>
       <c r="H31" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I31" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J31" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="K31" s="11"/>
-      <c r="L31" s="5">
+        <v>45</v>
+      </c>
+      <c r="J31" s="11"/>
+      <c r="K31" s="5">
         <v>3</v>
       </c>
-      <c r="M31" s="34">
-        <v>4</v>
-      </c>
-      <c r="N31" s="5">
+      <c r="L31" s="34">
+        <v>2</v>
+      </c>
+      <c r="M31" s="5">
         <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="O31" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="N31" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="P31" s="9"/>
+      <c r="O31" s="9"/>
       <c r="AI31" s="1"/>
       <c r="AJ31" s="1"/>
       <c r="AK31" s="1"/>
@@ -2847,21 +3016,49 @@
       <c r="AU31" s="1"/>
       <c r="AV31" s="1"/>
     </row>
-    <row r="32" spans="1:48" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
-      <c r="N32" s="3"/>
+    <row r="32" spans="1:48" ht="163.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="6">
+        <v>45391</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="H32" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="J32" s="11"/>
+      <c r="K32" s="5">
+        <v>4</v>
+      </c>
+      <c r="L32" s="34">
+        <v>3</v>
+      </c>
+      <c r="M32" s="5">
+        <f t="shared" ref="M32" si="4">K32*L32</f>
+        <v>12</v>
+      </c>
+      <c r="N32" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="O32" s="9"/>
       <c r="AI32" s="1"/>
       <c r="AJ32" s="1"/>
       <c r="AK32" s="1"/>
@@ -5759,24 +5956,24 @@
     </row>
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
-  <conditionalFormatting sqref="N3:N31">
+  <conditionalFormatting sqref="M3:M32">
     <cfRule type="iconSet" priority="3">
       <iconSet reverse="1">
         <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="4"/>
+        <cfvo type="num" val="7"/>
         <cfvo type="num" val="13"/>
       </iconSet>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:L31" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K32" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>1</formula1>
       <formula2>5</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B31" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B32" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>$Y$1:$AA$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y2 M3:M31" xr:uid="{11E2E0DE-B4FB-4EE6-8C7C-D4C3FCCE73CF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y2 L3:L32" xr:uid="{11E2E0DE-B4FB-4EE6-8C7C-D4C3FCCE73CF}">
       <formula1>$Y$2:$AC$2</formula1>
     </dataValidation>
   </dataValidations>
@@ -6203,7 +6400,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
@@ -6211,7 +6408,7 @@
         <v>13</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
@@ -6219,7 +6416,7 @@
         <v>14</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
@@ -6227,7 +6424,7 @@
         <v>15</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6255,7 +6452,7 @@
         <v>21</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
@@ -6263,7 +6460,7 @@
         <v>22</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
@@ -6271,7 +6468,7 @@
         <v>23</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6279,7 +6476,7 @@
         <v>24</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6300,17 +6497,17 @@
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" s="36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -6328,6 +6525,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101000B674BCD04104143B925E94D13EE63D6" ma:contentTypeVersion="8" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="02a8e9dbe448fde3d28822232c77ecba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v3/fields" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="99c78fe733576f46bbe313b297c8672b" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3/fields"/>
@@ -6453,15 +6659,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51D06A13-7C9B-4B18-BB8A-77CA0E1B2E6E}">
   <ds:schemaRefs>
@@ -6479,6 +6676,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA2A1C89-8A51-4743-A56F-F8C5CF25D0ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9024F26D-946A-4EA8-A6DE-31008C1E0148}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6494,12 +6699,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA2A1C89-8A51-4743-A56F-F8C5CF25D0ED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>